<commit_message>
fix: demand router switching
</commit_message>
<xml_diff>
--- a/fastapi-backend/air_passenger_yearly_2035.xlsx
+++ b/fastapi-backend/air_passenger_yearly_2035.xlsx
@@ -1,33 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research RTDA Project Bergamo\Project 1 Demand forecasting\Final datasets and codes 15_3_2024\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB1F07D-EC19-466F-8A9D-41902DC0790C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Passegger</t>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Passenger</t>
   </si>
   <si>
     <t>Forecasted</t>
@@ -44,20 +36,23 @@
   <si>
     <t>95%_upper</t>
   </si>
-  <si>
-    <t>Year</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -65,19 +60,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -85,9 +417,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -95,17 +669,61 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -154,7 +772,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,26 +805,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,23 +840,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,80 +1010,80 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.2166666666667" customWidth="1"/>
+    <col min="3" max="3" width="13.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>92.441619000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>92.441619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>90.209067000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>90.209067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>91.292485999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91.292486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>100.87376399999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100.873764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -507,15 +1091,15 @@
         <v>107.778431</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>113.33564800000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>113.335648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -523,47 +1107,47 @@
         <v>123.727412</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>136.19231500000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>136.192315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>133.79959099999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>133.799591</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>130.69192000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130.69192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>139.73674600000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>139.736746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>148.78142299999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>148.781423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -571,15 +1155,15 @@
         <v>146.885357</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>144.15194600000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>144.151946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -587,7 +1171,7 @@
         <v>150.505585</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -595,7 +1179,7 @@
         <v>157.07</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -603,23 +1187,23 @@
         <v>164.477812</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>175.34096500000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>175.340965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>185.61932999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>185.61933</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -627,23 +1211,23 @@
         <v>193.077517</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>52.904282000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52.904282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>80.659462172999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80.659462173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -651,87 +1235,87 @@
         <v>164.589799</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>2025</v>
       </c>
       <c r="C25">
-        <v>215.94934110741909</v>
+        <v>215.949341107419</v>
       </c>
       <c r="D25">
-        <v>194.17586877518721</v>
+        <v>194.175868775187</v>
       </c>
       <c r="E25">
-        <v>237.5488564600625</v>
+        <v>237.548856460062</v>
       </c>
       <c r="F25">
-        <v>184.96779499809591</v>
+        <v>184.967794998096</v>
       </c>
       <c r="G25">
-        <v>246.57002647806959</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>246.57002647807</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2026</v>
       </c>
       <c r="C26">
-        <v>225.83666148893579</v>
+        <v>225.836661488936</v>
       </c>
       <c r="D26">
-        <v>193.0417184693635</v>
+        <v>193.041718469364</v>
       </c>
       <c r="E26">
-        <v>257.5204162255738</v>
+        <v>257.520416225574</v>
       </c>
       <c r="F26">
-        <v>176.5165259628464</v>
+        <v>176.516525962846</v>
       </c>
       <c r="G26">
-        <v>273.52445133541761</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>273.524451335418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>2027</v>
       </c>
       <c r="C27">
-        <v>236.0232638548058</v>
+        <v>236.023263854806</v>
       </c>
       <c r="D27">
-        <v>201.12555381043919</v>
+        <v>201.125553810439</v>
       </c>
       <c r="E27">
-        <v>271.14614589747327</v>
+        <v>271.146145897473</v>
       </c>
       <c r="F27">
-        <v>179.28196817809271</v>
+        <v>179.281968178093</v>
       </c>
       <c r="G27">
-        <v>289.15973694072068</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>289.159736940721</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2028</v>
       </c>
       <c r="C28">
-        <v>245.27458916496511</v>
+        <v>245.274589164965</v>
       </c>
       <c r="D28">
         <v>208.766553918835</v>
       </c>
       <c r="E28">
-        <v>284.20598855985259</v>
+        <v>284.205988559853</v>
       </c>
       <c r="F28">
-        <v>187.13353505885109</v>
+        <v>187.133535058851</v>
       </c>
       <c r="G28">
-        <v>302.5686491226852</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>302.568649122685</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2029</v>
       </c>
@@ -739,139 +1323,140 @@
         <v>254.294447821896</v>
       </c>
       <c r="D29">
-        <v>216.2354521230998</v>
+        <v>216.2354521231</v>
       </c>
       <c r="E29">
-        <v>293.23149978458872</v>
+        <v>293.231499784589</v>
       </c>
       <c r="F29">
-        <v>194.86594592992611</v>
+        <v>194.865945929926</v>
       </c>
       <c r="G29">
-        <v>316.4937371266987</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>316.493737126699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2030</v>
       </c>
       <c r="C30">
-        <v>263.76425072120452</v>
+        <v>263.764250721205</v>
       </c>
       <c r="D30">
         <v>223.211691551576</v>
       </c>
       <c r="E30">
-        <v>305.88241311493732</v>
+        <v>305.882413114937</v>
       </c>
       <c r="F30">
         <v>202.316237987628</v>
       </c>
       <c r="G30">
-        <v>328.05401474325049</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>328.05401474325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>2031</v>
       </c>
       <c r="C31">
-        <v>272.98984133688413</v>
+        <v>272.989841336884</v>
       </c>
       <c r="D31">
-        <v>229.1288177719936</v>
+        <v>229.128817771994</v>
       </c>
       <c r="E31">
-        <v>317.86834254535358</v>
+        <v>317.868342545354</v>
       </c>
       <c r="F31">
-        <v>203.97165737957781</v>
+        <v>203.971657379578</v>
       </c>
       <c r="G31">
-        <v>339.06139032574742</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>339.061390325747</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>2032</v>
       </c>
       <c r="C32">
-        <v>283.40992131666388</v>
+        <v>283.409921316664</v>
       </c>
       <c r="D32">
-        <v>240.14244583656671</v>
+        <v>240.142445836567</v>
       </c>
       <c r="E32">
-        <v>328.57190144757789</v>
+        <v>328.571901447578</v>
       </c>
       <c r="F32">
-        <v>216.54522378205701</v>
+        <v>216.545223782057</v>
       </c>
       <c r="G32">
-        <v>356.08308905406068</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>356.083089054061</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>2033</v>
       </c>
       <c r="C33">
-        <v>293.28233599234079</v>
+        <v>293.282335992341</v>
       </c>
       <c r="D33">
-        <v>249.3513574177783</v>
+        <v>249.351357417778</v>
       </c>
       <c r="E33">
-        <v>340.90526735159978</v>
+        <v>340.9052673516</v>
       </c>
       <c r="F33">
-        <v>225.4286193446809</v>
+        <v>225.428619344681</v>
       </c>
       <c r="G33">
-        <v>360.78353011248089</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>360.783530112481</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>2034</v>
       </c>
       <c r="C34">
-        <v>302.03426778768102</v>
+        <v>302.034267787681</v>
       </c>
       <c r="D34">
         <v>252.56898394445</v>
       </c>
       <c r="E34">
-        <v>352.86596700414469</v>
+        <v>352.865967004145</v>
       </c>
       <c r="F34">
         <v>231.96748115915</v>
       </c>
       <c r="G34">
-        <v>376.78192260668681</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>376.781922606687</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>2035</v>
       </c>
       <c r="C35">
-        <v>311.29276164627038</v>
+        <v>311.29276164627</v>
       </c>
       <c r="D35">
-        <v>259.71801279839002</v>
+        <v>259.71801279839</v>
       </c>
       <c r="E35">
-        <v>363.10112451466642</v>
+        <v>363.101124514666</v>
       </c>
       <c r="F35">
-        <v>232.21784833839649</v>
+        <v>232.217848338396</v>
       </c>
       <c r="G35">
-        <v>390.11543810424109</v>
+        <v>390.115438104241</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>